<commit_message>
Prepare context data for survey rendering
</commit_message>
<xml_diff>
--- a/surveyapp/data/all_conversations.xlsx
+++ b/surveyapp/data/all_conversations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\Desktop\surveyapp\surveyapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74FFCD3-A08A-487C-AA15-C57ECE14B585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474BBB26-8855-4377-AB20-980B3253B9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="550" yWindow="1690" windowWidth="14010" windowHeight="7990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="550" yWindow="1690" windowWidth="16800" windowHeight="7990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
-    <t>file_name</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>ai</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -390,20 +390,20 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -411,10 +411,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -422,10 +422,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -433,10 +433,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -444,10 +444,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -455,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -466,10 +466,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -477,10 +477,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -488,10 +488,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register by email, small ui fixes
</commit_message>
<xml_diff>
--- a/surveyapp/data/all_conversations.xlsx
+++ b/surveyapp/data/all_conversations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\Desktop\surveyapp\surveyapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474BBB26-8855-4377-AB20-980B3253B9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A4C3F-AADF-4CE7-AAC0-16C29908DF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="550" yWindow="1690" windowWidth="16800" windowHeight="7990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>number</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__09_31_44</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__09_38_05</t>
   </si>
 </sst>
 </file>
@@ -387,13 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="44.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -492,6 +501,28 @@
       </c>
       <c r="C9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update start screen instructions, add ai generated conversations to data
</commit_message>
<xml_diff>
--- a/surveyapp/data/all_conversations.xlsx
+++ b/surveyapp/data/all_conversations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\Desktop\surveyapp\surveyapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7A4C3F-AADF-4CE7-AAC0-16C29908DF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D31262-F992-44D8-9AD7-27882D24952D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,58 +25,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>number</t>
   </si>
   <si>
-    <t>conv_1</t>
-  </si>
-  <si>
-    <t>conv_2</t>
-  </si>
-  <si>
-    <t>conv_3</t>
-  </si>
-  <si>
-    <t>conv_4</t>
-  </si>
-  <si>
-    <t>conv_5</t>
-  </si>
-  <si>
-    <t>conv_6</t>
-  </si>
-  <si>
-    <t>conv_7</t>
-  </si>
-  <si>
-    <t>conv_8</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
-    <t>human</t>
-  </si>
-  <si>
     <t>ai</t>
   </si>
   <si>
     <t>code</t>
   </si>
   <si>
-    <t>conversation_11_07_2023__09_31_44</t>
-  </si>
-  <si>
-    <t>conversation_11_07_2023__09_38_05</t>
+    <t>conversation_11_07_2023__14_39_52</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__14_45_34.</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__14_51_17</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__14_56_58</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__15_02_40</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__13_03_37</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__13_09_34</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__13_22_32</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__13_28_19</t>
+  </si>
+  <si>
+    <t>conversation_11_07_2023__13_37_20</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_24_09</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_31_31</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_39_56</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_47_14</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_53_17</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__09_59_29</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__10_11_06</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__10_17_00</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__10_22_51</t>
+  </si>
+  <si>
+    <t>conversation_12_07_2023__10_05_17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +116,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,140 +426,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>11</v>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>